<commit_message>
Made some changes to front-end. Beginning to test simple submission of Excel sheet.
</commit_message>
<xml_diff>
--- a/project/webapp/golang/testing-project/static/exampleFiles/ExampleSheet.xlsx
+++ b/project/webapp/golang/testing-project/static/exampleFiles/ExampleSheet.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Example Name</t>
   </si>
   <si>
-    <t xml:space="preserve">To your left is an example name, between 1 and 20 characters, a phone number with an area code and ten digits, and a ‘saying’ column that is between 1 and 120 characters!</t>
+    <t xml:space="preserve">Here is the example message. It must be between 1 and 120 characters!</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>